<commit_message>
attack on permutation not working, is it a bug?
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simbe\Desktop\Project\my\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simbe\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC04C8E2-CFFE-4020-A27C-0A62AD7E33B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A400F11B-A15C-44D8-A980-C0D406338CAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C375EEB-93F3-4E7E-9B74-48020E12308A}"/>
   </bookViews>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>mnist</t>
   </si>
   <si>
     <t>fashion_mnist</t>
-  </si>
-  <si>
-    <t>cifar10</t>
   </si>
   <si>
     <t>CW_1</t>
@@ -71,12 +68,18 @@
   <si>
     <t>PERMUTATED</t>
   </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>attacked</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +109,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -305,142 +315,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -757,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D8022F-5CAF-4859-A522-155D07086E77}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,581 +823,617 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="5.109375" customWidth="1"/>
-    <col min="4" max="8" width="12.77734375" customWidth="1"/>
+    <col min="4" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="19">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E2" s="19">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="56"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="22">
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="12">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E3" s="22">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="12">
+        <v>100</v>
+      </c>
+      <c r="F3" s="12">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="E4" s="11">
-        <v>10.62</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="48"/>
+      <c r="B4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="25">
-        <v>3.5</v>
-      </c>
-      <c r="E5" s="26">
-        <v>12.33</v>
-      </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="48"/>
+      <c r="D5" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7">
+        <v>10.62</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="22">
-        <v>3.37</v>
-      </c>
-      <c r="E6" s="29">
-        <v>13.1</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="49"/>
+      <c r="D6" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="19">
+        <v>3.7</v>
+      </c>
+      <c r="F6" s="19">
+        <v>12.33</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="11">
-        <v>3.02</v>
-      </c>
-      <c r="E7" s="12">
-        <v>12.04</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="48"/>
+      <c r="B7" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="50"/>
+      <c r="D7" s="15">
+        <v>3.37</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22">
+        <v>13.1</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="56"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="31">
-        <v>16.579999999999998</v>
-      </c>
-      <c r="E8" s="32">
-        <v>55.66</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="7">
+        <v>3.02</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
+        <v>12.04</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="56"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="34">
-        <v>18.11</v>
-      </c>
-      <c r="E9" s="35">
-        <v>41.97</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23">
+        <v>16.579999999999998</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="43">
+        <v>55.66</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="36" t="s">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="48"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="37">
-        <v>16.71</v>
-      </c>
-      <c r="E10" s="38">
-        <v>55.35</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="D10" s="25">
+        <v>18.11</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="40">
+        <v>41.97</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="34">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="E11" s="35">
-        <v>41.47</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="48"/>
+      <c r="B11" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="27">
+        <v>16.71</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="41">
+        <v>55.35</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="36" t="s">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="37">
-        <v>20.88</v>
-      </c>
-      <c r="E12" s="38">
-        <v>59.23</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="25">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="40">
+        <v>41.47</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="17">
-        <v>19.95</v>
-      </c>
-      <c r="E13" s="13">
-        <v>46.25</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27">
+        <v>20.88</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="41">
+        <v>59.23</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="30" t="s">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="48"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="40">
-        <v>64.069999999999993</v>
-      </c>
-      <c r="E14" s="32">
-        <v>72.12</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="D14" s="10">
+        <v>19.95</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="45">
+        <v>46.25</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="15">
-        <v>69.12</v>
-      </c>
-      <c r="E15" s="35">
-        <v>64.47</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="37">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="43">
+        <v>72.12</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="56"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="36" t="s">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="48"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="41">
-        <v>63.76</v>
-      </c>
-      <c r="E16" s="38">
-        <v>90</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="D16" s="38">
+        <v>69.12</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="40">
+        <v>64.47</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="35">
-        <v>88.65</v>
-      </c>
-      <c r="E17" s="35">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="48"/>
+      <c r="B17" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="39">
+        <v>63.76</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="41">
         <v>90</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="56"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="42" t="s">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="48"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="40">
         <v>88.65</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="26"/>
+      <c r="F18" s="40">
         <v>90</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="41">
         <v>88.65</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="28"/>
+      <c r="F19" s="41">
         <v>90</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="43" t="s">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="42">
         <v>88.65</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="9"/>
+      <c r="F20" s="45">
         <v>90</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="35">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="43">
         <v>88.65</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="24"/>
+      <c r="F21" s="43">
         <v>90</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="56"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="42" t="s">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="48"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="40">
         <v>88.65</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="26"/>
+      <c r="F22" s="40">
         <v>90</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="56"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="38">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="48"/>
+      <c r="B23" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="41">
         <v>88.65</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="28"/>
+      <c r="F23" s="41">
         <v>90</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="56"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="42" t="s">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="41">
         <v>88.65</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="28"/>
+      <c r="F24" s="41">
         <v>90</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="14">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="48"/>
+      <c r="B25" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="41">
         <v>88.65</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="28"/>
+      <c r="F25" s="41">
         <v>90</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="44">
+        <v>88.65</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="45">
+        <v>90</v>
+      </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1353,11 +1444,12 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1368,11 +1460,12 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1383,8 +1476,9 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1398,8 +1492,9 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1413,8 +1508,9 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1428,8 +1524,9 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1443,8 +1540,9 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1458,8 +1556,9 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1473,30 +1572,49 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A3:A5"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
started working on poster
</commit_message>
<xml_diff>
--- a/accuracies.xlsx
+++ b/accuracies.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simbe\Desktop\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF58F8A9-5DE2-4C66-87A4-852C991FB9E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="30">
   <si>
     <t>mnist</t>
   </si>
@@ -102,12 +108,6 @@
     </r>
   </si>
   <si>
-    <t>encrypt v1</t>
-  </si>
-  <si>
-    <t>encrypt v2</t>
-  </si>
-  <si>
     <t>28x28</t>
   </si>
   <si>
@@ -175,12 +175,45 @@
 [ 10.000 samples - CW model ]</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>42</t>
+    </r>
+  </si>
+  <si>
+    <t>future work</t>
+  </si>
+  <si>
+    <t>flattening</t>
+  </si>
+  <si>
+    <t>blocking</t>
+  </si>
+  <si>
+    <t>fashion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +303,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -279,7 +318,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -710,19 +749,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -763,11 +789,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,7 +890,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -826,12 +897,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -890,12 +955,12 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,7 +985,177 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -945,154 +1180,50 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="140"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="140"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="140"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="140"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="140"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="140"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1401,56 +1532,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="72" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="108" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="72" t="s">
+      <c r="E2" s="88"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="92"/>
       <c r="J2" s="4"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1458,24 +1589,24 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="70" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="70" t="s">
+      <c r="F3" s="93"/>
+      <c r="G3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="76"/>
+      <c r="I3" s="93"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1483,23 +1614,23 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="71"/>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="77"/>
+      <c r="H4" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>23</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1508,28 +1639,28 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="63">
+      <c r="C5" s="105"/>
+      <c r="D5" s="72">
         <v>1.49</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="114">
         <v>100</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63">
+      <c r="F5" s="115"/>
+      <c r="G5" s="72">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="114">
         <v>100</v>
       </c>
-      <c r="I5" s="62"/>
+      <c r="I5" s="115"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1537,22 +1668,22 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="75"/>
-      <c r="B6" s="95" t="s">
+    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="84"/>
+      <c r="B6" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="57">
+      <c r="C6" s="107"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="110">
         <v>100</v>
       </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="57">
+      <c r="F6" s="111"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="110">
         <v>100</v>
       </c>
-      <c r="I6" s="58"/>
+      <c r="I6" s="111"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1560,22 +1691,22 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
-      <c r="B7" s="102" t="s">
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="84"/>
+      <c r="B7" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="57">
+      <c r="C7" s="81"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="110">
         <v>100</v>
       </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="57">
+      <c r="F7" s="111"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="110">
         <v>100</v>
       </c>
-      <c r="I7" s="58"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1583,26 +1714,26 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="87"/>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="30">
+      <c r="C8" s="83"/>
+      <c r="D8" s="27">
         <v>2.1</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="112">
         <v>82.94</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="30">
+      <c r="F8" s="113"/>
+      <c r="G8" s="27">
         <v>9.5</v>
       </c>
-      <c r="H8" s="59">
+      <c r="H8" s="112">
         <v>94.25</v>
       </c>
-      <c r="I8" s="60"/>
+      <c r="I8" s="113"/>
       <c r="J8" s="7"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1610,30 +1741,30 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="s">
+    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="63">
+      <c r="C9" s="105"/>
+      <c r="D9" s="72">
         <v>3.7</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="28">
         <v>100</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="29">
         <v>4.5</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="72">
         <v>12.3</v>
       </c>
-      <c r="H9" s="112">
+      <c r="H9" s="60">
         <v>100</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="29">
         <v>12.7</v>
       </c>
       <c r="J9" s="1"/>
@@ -1643,24 +1774,24 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="89" t="s">
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="84"/>
+      <c r="B10" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="33">
+      <c r="C10" s="93"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="30">
         <v>100</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="30">
         <v>7.3</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="33">
+      <c r="G10" s="72"/>
+      <c r="H10" s="30">
         <v>100</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="30">
         <v>12.5</v>
       </c>
       <c r="J10" s="1"/>
@@ -1670,24 +1801,24 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="102" t="s">
+    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="84"/>
+      <c r="B11" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="33">
+      <c r="C11" s="81"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="30">
         <v>100</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="31">
         <v>5.4</v>
       </c>
-      <c r="G11" s="64"/>
-      <c r="H11" s="33">
+      <c r="G11" s="73"/>
+      <c r="H11" s="30">
         <v>100</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="31">
         <v>12.9</v>
       </c>
       <c r="J11" s="1"/>
@@ -1697,28 +1828,28 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="87"/>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="94"/>
-      <c r="D12" s="30">
+      <c r="C12" s="83"/>
+      <c r="D12" s="27">
         <v>4.1900000000000004</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="27">
         <v>81.400000000000006</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="27">
         <v>53.4</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="27">
         <v>12</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="32">
         <v>89.7</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="27">
         <v>72.599999999999994</v>
       </c>
       <c r="J12" s="1"/>
@@ -1728,29 +1859,33 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="86" t="s">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="90" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="36">
+        <v>27</v>
+      </c>
+      <c r="D13" s="33">
         <v>16.579999999999998</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37">
+      <c r="E13" s="117" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="34">
         <v>55.66</v>
       </c>
-      <c r="H13" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="65" t="s">
-        <v>22</v>
+      <c r="H13" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="74" t="s">
+        <v>20</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1759,22 +1894,22 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="90"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="84"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="38">
+        <v>28</v>
+      </c>
+      <c r="D14" s="35">
         <v>18.11</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39">
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="36">
         <v>41.97</v>
       </c>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
       <c r="J14" s="7"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1782,24 +1917,24 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="89" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="84"/>
+      <c r="B15" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="40">
+        <v>27</v>
+      </c>
+      <c r="D15" s="37">
         <v>20.88</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="41">
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="38">
         <v>59.23</v>
       </c>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="7"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1807,22 +1942,22 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="88"/>
-      <c r="B16" s="89"/>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="85"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="42">
+        <v>28</v>
+      </c>
+      <c r="D16" s="39">
         <v>19.95</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43">
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="40">
         <v>46.25</v>
       </c>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1830,33 +1965,33 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="44">
+      <c r="C17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="41">
         <v>64.069999999999993</v>
       </c>
-      <c r="E17" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="45">
+      <c r="E17" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="42">
         <v>72.12</v>
       </c>
-      <c r="H17" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="67" t="s">
-        <v>22</v>
+      <c r="H17" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="69" t="s">
+        <v>20</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1865,22 +2000,22 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="90"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="84"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="39">
+        <v>28</v>
+      </c>
+      <c r="D18" s="36">
         <v>69.12</v>
       </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="41">
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="38">
         <v>64.47</v>
       </c>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1888,24 +2023,24 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="89" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="84"/>
+      <c r="B19" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="41">
+        <v>27</v>
+      </c>
+      <c r="D19" s="38">
         <v>88.65</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="41">
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="38">
         <v>90</v>
       </c>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1913,22 +2048,22 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="87"/>
-      <c r="B20" s="93"/>
-      <c r="C20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="46">
+      <c r="B20" s="82"/>
+      <c r="C20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="43">
         <v>88.65</v>
       </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="47">
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="44">
         <v>90</v>
       </c>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1936,33 +2071,33 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75" t="s">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="90" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="37">
+        <v>27</v>
+      </c>
+      <c r="D21" s="34">
         <v>88.65</v>
       </c>
-      <c r="E21" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="37">
+      <c r="E21" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="34">
         <v>90</v>
       </c>
-      <c r="H21" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="65" t="s">
-        <v>22</v>
+      <c r="H21" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="74" t="s">
+        <v>20</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="1"/>
@@ -1971,22 +2106,22 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
-      <c r="B22" s="90"/>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="84"/>
+      <c r="B22" s="89"/>
       <c r="C22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="39">
+        <v>28</v>
+      </c>
+      <c r="D22" s="36">
         <v>88.65</v>
       </c>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="43">
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="40">
         <v>90</v>
       </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="7"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1994,24 +2129,24 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="75"/>
-      <c r="B23" s="89" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="84"/>
+      <c r="B23" s="90" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="41">
+        <v>27</v>
+      </c>
+      <c r="D23" s="38">
         <v>88.65</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="41">
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="38">
         <v>90</v>
       </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
       <c r="J23" s="7"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2019,22 +2154,22 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="88"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="48">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="85"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="45">
         <v>88.65</v>
       </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="48">
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="45">
         <v>90</v>
       </c>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
       <c r="J24" s="7"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2042,16 +2177,16 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -2059,16 +2194,16 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -2076,7 +2211,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2093,10 +2228,10 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2110,17 +2245,17 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+    <row r="29" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2129,17 +2264,17 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="98" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="99"/>
-      <c r="D30" s="25" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="79"/>
+      <c r="D30" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>20</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="16"/>
@@ -2152,18 +2287,18 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="106" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="100" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="50">
+      <c r="B31" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="62"/>
+      <c r="D31" s="47">
         <v>3.63</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="23">
         <v>4</v>
       </c>
       <c r="F31" s="16"/>
@@ -2177,13 +2312,13 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="100" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="101"/>
-      <c r="D32" s="51">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="66"/>
+      <c r="B32" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="62"/>
+      <c r="D32" s="48">
         <v>2.65</v>
       </c>
       <c r="E32" s="17">
@@ -2200,16 +2335,16 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="50">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="66"/>
+      <c r="B33" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="62"/>
+      <c r="D33" s="47">
         <v>2.69</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="20">
         <v>12</v>
       </c>
       <c r="F33" s="15"/>
@@ -2223,13 +2358,13 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
-      <c r="B34" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="52">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="67"/>
+      <c r="B34" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="61"/>
+      <c r="D34" s="49">
         <v>2.2999999999999998</v>
       </c>
       <c r="E34" s="17">
@@ -2246,18 +2381,20 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="106" t="s">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="100" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="53">
+      <c r="B35" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="62"/>
+      <c r="D35" s="50">
         <v>12.4</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="20">
+        <v>5</v>
+      </c>
       <c r="F35" s="15"/>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
@@ -2269,16 +2406,16 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
-      <c r="B36" s="109" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="101"/>
-      <c r="D36" s="50">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="66"/>
+      <c r="B36" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="62"/>
+      <c r="D36" s="47">
         <v>12.07</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="20">
         <v>13</v>
       </c>
       <c r="F36" s="15"/>
@@ -2292,61 +2429,661 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
-      <c r="B37" s="104" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="105"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19"/>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="67"/>
+      <c r="B37" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="64"/>
+      <c r="D37" s="116">
+        <v>11.41</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="18"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="108"/>
-      <c r="B38" s="104" t="s">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="105"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="108"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="108"/>
+      <c r="I48" s="108"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="94"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="88"/>
+      <c r="F49" s="92"/>
+      <c r="G49" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="H49" s="88"/>
+      <c r="I49" s="92"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="97"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="99"/>
+      <c r="D50" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="93"/>
+      <c r="G50" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" s="93"/>
+    </row>
+    <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="100"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="102"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="77"/>
+      <c r="H51" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="105"/>
+      <c r="D52" s="72">
+        <v>1.49</v>
+      </c>
+      <c r="E52" s="114">
+        <v>100</v>
+      </c>
+      <c r="F52" s="115"/>
+      <c r="G52" s="72">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H52" s="114">
+        <v>100</v>
+      </c>
+      <c r="I52" s="115"/>
+    </row>
+    <row r="53" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="84"/>
+      <c r="B53" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="107"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="110">
+        <v>100</v>
+      </c>
+      <c r="F53" s="111"/>
+      <c r="G53" s="72"/>
+      <c r="H53" s="110">
+        <v>100</v>
+      </c>
+      <c r="I53" s="111"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="84"/>
+      <c r="B54" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="81"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="110">
+        <v>100</v>
+      </c>
+      <c r="F54" s="111"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="110">
+        <v>100</v>
+      </c>
+      <c r="I54" s="111"/>
+    </row>
+    <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="87"/>
+      <c r="B55" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="83"/>
+      <c r="D55" s="27">
+        <v>2.1</v>
+      </c>
+      <c r="E55" s="112">
+        <v>82.94</v>
+      </c>
+      <c r="F55" s="113"/>
+      <c r="G55" s="27">
+        <v>9.5</v>
+      </c>
+      <c r="H55" s="112">
+        <v>94.25</v>
+      </c>
+      <c r="I55" s="113"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="105"/>
+      <c r="D56" s="72">
+        <v>3.7</v>
+      </c>
+      <c r="E56" s="51">
+        <v>100</v>
+      </c>
+      <c r="F56" s="29">
+        <v>4.5</v>
+      </c>
+      <c r="G56" s="72">
+        <v>12.3</v>
+      </c>
+      <c r="H56" s="60">
+        <v>100</v>
+      </c>
+      <c r="I56" s="29">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="84"/>
+      <c r="B57" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="93"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="30">
+        <v>100</v>
+      </c>
+      <c r="F57" s="30">
+        <v>7.3</v>
+      </c>
+      <c r="G57" s="72"/>
+      <c r="H57" s="30">
+        <v>100</v>
+      </c>
+      <c r="I57" s="30">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="84"/>
+      <c r="B58" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="81"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="30">
+        <v>100</v>
+      </c>
+      <c r="F58" s="52">
+        <v>5.4</v>
+      </c>
+      <c r="G58" s="73"/>
+      <c r="H58" s="30">
+        <v>100</v>
+      </c>
+      <c r="I58" s="52">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59" s="85"/>
+      <c r="B59" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="120"/>
+      <c r="D59" s="118">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E59" s="118">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="F59" s="118">
+        <v>53.4</v>
+      </c>
+      <c r="G59" s="118">
+        <v>12</v>
+      </c>
+      <c r="H59" s="119">
+        <v>89.7</v>
+      </c>
+      <c r="I59" s="118">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60" s="55"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="123"/>
+      <c r="E60" s="123"/>
+      <c r="F60" s="123"/>
+      <c r="G60" s="123"/>
+      <c r="H60" s="123"/>
+      <c r="I60" s="123"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61" s="55"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="123"/>
+      <c r="E61" s="123"/>
+      <c r="F61" s="123"/>
+      <c r="G61" s="123"/>
+      <c r="H61" s="123"/>
+      <c r="I61" s="123"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="56"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="123"/>
+      <c r="E62" s="123"/>
+      <c r="F62" s="123"/>
+      <c r="G62" s="123"/>
+      <c r="H62" s="123"/>
+      <c r="I62" s="123"/>
+    </row>
+    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="128"/>
+      <c r="B63" s="126"/>
+      <c r="C63" s="127"/>
+      <c r="D63" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="130"/>
+      <c r="G63" s="129"/>
+    </row>
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="103" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="33">
+        <v>16.579999999999998</v>
+      </c>
+      <c r="E64" s="34">
+        <v>55.66</v>
+      </c>
+      <c r="F64" s="122"/>
+      <c r="G64" s="122"/>
+      <c r="H64" s="122"/>
+      <c r="I64" s="122"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="84"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="35">
+        <v>18.11</v>
+      </c>
+      <c r="E65" s="36">
+        <v>41.97</v>
+      </c>
+      <c r="F65" s="122"/>
+      <c r="G65" s="122"/>
+      <c r="H65" s="122"/>
+      <c r="I65" s="122"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="84"/>
+      <c r="B66" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="37">
+        <v>20.88</v>
+      </c>
+      <c r="E66" s="38">
+        <v>59.23</v>
+      </c>
+      <c r="F66" s="122"/>
+      <c r="G66" s="122"/>
+      <c r="H66" s="122"/>
+      <c r="I66" s="122"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+    </row>
+    <row r="67" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="87"/>
+      <c r="B67" s="82"/>
+      <c r="C67" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="131">
+        <v>19.95</v>
+      </c>
+      <c r="E67" s="43">
+        <v>46.25</v>
+      </c>
+      <c r="F67" s="122"/>
+      <c r="G67" s="122"/>
+      <c r="H67" s="122"/>
+      <c r="I67" s="122"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+    </row>
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="36">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="E68" s="40">
+        <v>72.12</v>
+      </c>
+      <c r="F68" s="122"/>
+      <c r="G68" s="122"/>
+      <c r="H68" s="121"/>
+      <c r="I68" s="122"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="84"/>
+      <c r="B69" s="89"/>
+      <c r="C69" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="36">
+        <v>69.12</v>
+      </c>
+      <c r="E69" s="38">
+        <v>64.47</v>
+      </c>
+      <c r="F69" s="122"/>
+      <c r="G69" s="122"/>
+      <c r="H69" s="122"/>
+      <c r="I69" s="122"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="84"/>
+      <c r="B70" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="38">
+        <v>88.65</v>
+      </c>
+      <c r="E70" s="38">
+        <v>90</v>
+      </c>
+      <c r="F70" s="122"/>
+      <c r="G70" s="122"/>
+      <c r="H70" s="122"/>
+      <c r="I70" s="122"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+    </row>
+    <row r="71" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="87"/>
+      <c r="B71" s="82"/>
+      <c r="C71" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="43">
+        <v>88.65</v>
+      </c>
+      <c r="E71" s="44">
+        <v>90</v>
+      </c>
+      <c r="F71" s="122"/>
+      <c r="G71" s="122"/>
+      <c r="H71" s="122"/>
+      <c r="I71" s="122"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+    </row>
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="34">
+        <v>88.65</v>
+      </c>
+      <c r="E72" s="34">
+        <v>90</v>
+      </c>
+      <c r="F72" s="122"/>
+      <c r="G72" s="122"/>
+      <c r="H72" s="122"/>
+      <c r="I72" s="122"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73" s="84"/>
+      <c r="B73" s="89"/>
+      <c r="C73" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" s="36">
+        <v>88.65</v>
+      </c>
+      <c r="E73" s="36">
+        <v>90</v>
+      </c>
+      <c r="F73" s="122"/>
+      <c r="G73" s="122"/>
+      <c r="H73" s="122"/>
+      <c r="I73" s="122"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" s="84"/>
+      <c r="B74" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="38">
+        <v>88.65</v>
+      </c>
+      <c r="E74" s="38">
+        <v>90</v>
+      </c>
+      <c r="F74" s="122"/>
+      <c r="G74" s="122"/>
+      <c r="H74" s="122"/>
+      <c r="I74" s="122"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" s="85"/>
+      <c r="B75" s="91"/>
+      <c r="C75" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="45">
+        <v>88.65</v>
+      </c>
+      <c r="E75" s="45">
+        <v>90</v>
+      </c>
+      <c r="F75" s="122"/>
+      <c r="G75" s="122"/>
+      <c r="H75" s="122"/>
+      <c r="I75" s="122"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C76" s="125"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
+  <mergeCells count="102">
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A49:C51"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="A2:C4"/>
@@ -2363,22 +3100,36 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>